<commit_message>
Close #44 - Notifications Controller
</commit_message>
<xml_diff>
--- a/core/excel/Test.xlsx
+++ b/core/excel/Test.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="50">
   <si>
     <t>ID</t>
   </si>
@@ -166,6 +166,18 @@
   </si>
   <si>
     <t>Wed May 23 23:18:05 ART 2018</t>
+  </si>
+  <si>
+    <t>Wed May 23 02:07:40 ART 2018</t>
+  </si>
+  <si>
+    <t>Thu May 24 02:07:40 ART 2018</t>
+  </si>
+  <si>
+    <t>Wed May 23 02:07:42 ART 2018</t>
+  </si>
+  <si>
+    <t>Thu May 24 02:07:42 ART 2018</t>
   </si>
 </sst>
 </file>
@@ -771,7 +783,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -967,6 +979,57 @@
       </c>
       <c r="E11" t="s">
         <v>45</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" t="s">
+        <v>46</v>
+      </c>
+      <c r="E12" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" t="s">
+        <v>48</v>
+      </c>
+      <c r="E13" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" t="s">
+        <v>48</v>
+      </c>
+      <c r="E14" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Close - #43 - Test DAO's
- Added Dao's objects tests.
- Modified some Entities and Models test for 99% coverage.
- Commented 'setActiveAlarms(List)' method. It was duplicated.
</commit_message>
<xml_diff>
--- a/core/excel/Test.xlsx
+++ b/core/excel/Test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christian\Desktop\Facultad\Proyecto Profesional II\PP2-Project\administrador-herramientas-java\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christian\Desktop\Facultad\Proyecto Profesional II\PP2-Project\administrador-herramientas-java\core\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="37">
   <si>
     <t>ID</t>
   </si>
@@ -135,37 +135,10 @@
     <t>1</t>
   </si>
   <si>
-    <t>Tue May 22 22:52:24 GMT-03:00 2018</t>
-  </si>
-  <si>
-    <t>Wed May 23 22:52:24 GMT-03:00 2018</t>
-  </si>
-  <si>
-    <t>Tue May 22 23:08:24 GMT-03:00 2018</t>
-  </si>
-  <si>
-    <t>Wed May 23 23:08:24 GMT-03:00 2018</t>
-  </si>
-  <si>
-    <t>Pepe</t>
-  </si>
-  <si>
-    <t>Tue May 22 23:08:28 GMT-03:00 2018</t>
-  </si>
-  <si>
-    <t>Wed May 23 23:08:28 GMT-03:00 2018</t>
-  </si>
-  <si>
-    <t>Tue May 22 23:18:04 ART 2018</t>
-  </si>
-  <si>
-    <t>Wed May 23 23:18:04 ART 2018</t>
-  </si>
-  <si>
-    <t>Tue May 22 23:18:05 ART 2018</t>
-  </si>
-  <si>
-    <t>Wed May 23 23:18:05 ART 2018</t>
+    <t>Wed May 23 13:38:51 GMT-03:00 2018</t>
+  </si>
+  <si>
+    <t>Thu May 24 13:38:51 GMT-03:00 2018</t>
   </si>
 </sst>
 </file>
@@ -771,7 +744,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -833,7 +806,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="14.25" r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -878,10 +851,10 @@
         <v>22</v>
       </c>
       <c r="D6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7">
@@ -889,84 +862,16 @@
         <v>33</v>
       </c>
       <c r="B7" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C7" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="D7" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E7" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s">
-        <v>33</v>
-      </c>
-      <c r="B8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8" t="s">
-        <v>39</v>
-      </c>
-      <c r="D8" t="s">
-        <v>40</v>
-      </c>
-      <c r="E8" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B9" t="s">
-        <v>33</v>
-      </c>
-      <c r="C9" t="s">
-        <v>39</v>
-      </c>
-      <c r="D9" t="s">
-        <v>42</v>
-      </c>
-      <c r="E9" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="s">
-        <v>33</v>
-      </c>
-      <c r="B10" t="s">
-        <v>33</v>
-      </c>
-      <c r="C10" t="s">
-        <v>39</v>
-      </c>
-      <c r="D10" t="s">
-        <v>44</v>
-      </c>
-      <c r="E10" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="s">
-        <v>33</v>
-      </c>
-      <c r="B11" t="s">
-        <v>34</v>
-      </c>
-      <c r="C11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" t="s">
-        <v>44</v>
-      </c>
-      <c r="E11" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Close	#45 - Create setNumberLoan method
+ Added GetLastFreeNumberLoan method in LoanDAO;
+ Added testGetLastFreeNumberLoan() method in LoanDAOTest;
+ Added setLastLoanNumber() method in LoanSystem;
+ Added loanSystem.setLastLoanNumber() line in App;
</commit_message>
<xml_diff>
--- a/core/excel/Test.xlsx
+++ b/core/excel/Test.xlsx
@@ -135,10 +135,10 @@
     <t>1</t>
   </si>
   <si>
-    <t>Wed May 23 13:38:51 GMT-03:00 2018</t>
-  </si>
-  <si>
-    <t>Thu May 24 13:38:51 GMT-03:00 2018</t>
+    <t>Wed May 23 16:27:54 GMT-03:00 2018</t>
+  </si>
+  <si>
+    <t>Thu May 24 16:27:54 GMT-03:00 2018</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Close #49 - DAO's Refactor
- Refactor applied to all DAO's
- Tests updated
- Modified excel variable names to match spanish
</commit_message>
<xml_diff>
--- a/core/excel/Test.xlsx
+++ b/core/excel/Test.xlsx
@@ -1,34 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent>
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christian\Desktop\Facultad\Proyecto Profesional II\PP2-Project\administrador-herramientas-java\core\excel\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView activeTab="3" windowHeight="7620" windowWidth="20490" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="3" windowHeight="11595" windowWidth="25755" xWindow="360" yWindow="30"/>
   </bookViews>
   <sheets>
     <sheet name="Tools" r:id="rId1" sheetId="1"/>
     <sheet name="Supplies" r:id="rId2" sheetId="3"/>
     <sheet name="Borrowers" r:id="rId3" sheetId="4"/>
     <sheet name="Loans" r:id="rId4" sheetId="5"/>
-    <sheet name="ToolTypes" r:id="rId5" sheetId="2"/>
+    <sheet name="TipoHerramienta" r:id="rId5" sheetId="2"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="100">
   <si>
     <t>ID</t>
   </si>
@@ -129,49 +119,547 @@
     <t>Wed May 23 16:42:08 GMT-03:00 2018</t>
   </si>
   <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>Wed May 23 16:12:00 GMT-03:00 2018</t>
+  </si>
+  <si>
+    <t>Thu May 24 16:12:00 GMT-03:00 2018</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>Wed May 23 16:12:14 GMT-03:00 2018</t>
+  </si>
+  <si>
+    <t>Thu May 24 16:12:14 GMT-03:00 2018</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>Wed May 23 16:12:36 GMT-03:00 2018</t>
+  </si>
+  <si>
+    <t>Thu May 24 16:12:36 GMT-03:00 2018</t>
+  </si>
+  <si>
+    <t>Wed May 23 16:12:42 GMT-03:00 2018</t>
+  </si>
+  <si>
+    <t>Thu May 24 16:12:42 GMT-03:00 2018</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>Wed May 23 16:49:17 ART 2018</t>
+  </si>
+  <si>
+    <t>Thu May 24 16:49:17 ART 2018</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>Wed May 23 16:53:41 ART 2018</t>
+  </si>
+  <si>
+    <t>Thu May 24 16:53:41 ART 2018</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>Wed May 23 18:38:36 ART 2018</t>
+  </si>
+  <si>
+    <t>Thu May 24 18:38:36 ART 2018</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>Wed May 23 18:38:39 ART 2018</t>
+  </si>
+  <si>
+    <t>Thu May 24 18:38:39 ART 2018</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>Tue May 29 11:22:31 ART 2018</t>
+  </si>
+  <si>
+    <t>Wed May 30 11:22:31 ART 2018</t>
+  </si>
+  <si>
+    <t>Nombre</t>
+  </si>
+  <si>
+    <t>Vegeta</t>
+  </si>
+  <si>
+    <t>Tipo de herramienta</t>
+  </si>
+  <si>
+    <t>Nombre</t>
+  </si>
+  <si>
+    <t>Numero</t>
+  </si>
+  <si>
+    <t>Herramienta</t>
+  </si>
+  <si>
+    <t>Trabajador</t>
+  </si>
+  <si>
+    <t>Fecha</t>
+  </si>
+  <si>
+    <t>Expiracion</t>
+  </si>
+  <si>
+    <t>Nombre</t>
+  </si>
+  <si>
     <t>0</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>Wed May 23 16:27:54 GMT-03:00 2018</t>
-  </si>
-  <si>
-    <t>Thu May 24 16:27:54 GMT-03:00 2018</t>
+    <t>Tue May 29 14:01:15 ART 2018</t>
+  </si>
+  <si>
+    <t>Wed May 30 14:01:15 ART 2018</t>
+  </si>
+  <si>
+    <t>Tue May 29 14:01:16 ART 2018</t>
+  </si>
+  <si>
+    <t>Wed May 30 14:01:16 ART 2018</t>
+  </si>
+  <si>
+    <t>Tue May 29 14:03:03 ART 2018</t>
+  </si>
+  <si>
+    <t>Wed May 30 14:03:03 ART 2018</t>
+  </si>
+  <si>
+    <t>Tue May 29 14:03:04 ART 2018</t>
+  </si>
+  <si>
+    <t>Wed May 30 14:03:04 ART 2018</t>
+  </si>
+  <si>
+    <t>Tue May 29 15:53:51 ART 2018</t>
+  </si>
+  <si>
+    <t>Wed May 30 15:53:51 ART 2018</t>
+  </si>
+  <si>
+    <t>Tue May 29 15:53:52 ART 2018</t>
+  </si>
+  <si>
+    <t>Wed May 30 15:53:52 ART 2018</t>
+  </si>
+  <si>
+    <t>Tue May 29 15:53:53 ART 2018</t>
+  </si>
+  <si>
+    <t>Wed May 30 15:53:53 ART 2018</t>
+  </si>
+  <si>
+    <t>Tue May 29 16:02:11 ART 2018</t>
+  </si>
+  <si>
+    <t>Wed May 30 16:02:11 ART 2018</t>
+  </si>
+  <si>
+    <t>Tue May 29 16:02:12 ART 2018</t>
+  </si>
+  <si>
+    <t>Wed May 30 16:02:12 ART 2018</t>
+  </si>
+  <si>
+    <t>Tue May 29 16:03:08 ART 2018</t>
+  </si>
+  <si>
+    <t>Wed May 30 16:03:08 ART 2018</t>
+  </si>
+  <si>
+    <t>Tue May 29 16:03:09 ART 2018</t>
+  </si>
+  <si>
+    <t>Wed May 30 16:03:09 ART 2018</t>
+  </si>
+  <si>
+    <t>Tue May 29 17:01:50 ART 2018</t>
+  </si>
+  <si>
+    <t>Wed May 30 17:01:50 ART 2018</t>
+  </si>
+  <si>
+    <t>Tue May 29 17:01:51 ART 2018</t>
+  </si>
+  <si>
+    <t>Wed May 30 17:01:51 ART 2018</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
-    <font>
-      <sz val="11"/>
+  <fonts count="21">
+    <font>
+      <sz val="11.0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <u/>
-      <sz val="11"/>
+      <sz val="11.0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11.0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+      <color theme="10"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11.0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+      <color theme="11"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+      <color rgb="FFFF0000"/>
+    </font>
+    <font>
+      <sz val="18.0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+      <color theme="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15.0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+      <color theme="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13.0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+      <color theme="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11.0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+      <color theme="3"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+      <color rgb="FF3F3F76"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11.0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+      <color rgb="FF3F3F3F"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11.0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+      <color rgb="FFFA7D00"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11.0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+      <color rgb="FFFFFFFF"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+      <color rgb="FFFA7D00"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+      <color theme="1"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+      <color rgb="FF006100"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+      <color rgb="FF9C0006"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+      <color rgb="FF9C6500"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+      <color theme="0"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+      <color theme="1"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11.0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+      <color rgb="FF7F7F7F"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
+      <patternFill patternType="gray125">
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799980"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599990"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399980"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799980"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599990"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399980"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799980"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599990"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399980"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799980"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599990"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399980"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799980"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599990"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399980"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799980"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599990"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399980"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -179,23 +667,212 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <bottom style="thick">
+        <color rgb="FFACCCEA"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <bottom style="medium">
+        <color theme="4" tint="0.399980"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="43"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="7"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="9"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="41"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="5"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf applyAlignment="0" applyFont="0" applyNumberFormat="0" applyProtection="0" borderId="1" fillId="2" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="4" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="5" numFmtId="0"/>
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="2" fillId="0" fontId="6" numFmtId="0"/>
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="3" fillId="0" fontId="7" numFmtId="0"/>
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="4" fillId="0" fontId="8" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="8" numFmtId="0"/>
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="5" fillId="3" fontId="9" numFmtId="0"/>
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="6" fillId="4" fontId="10" numFmtId="0"/>
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="5" fillId="4" fontId="11" numFmtId="0"/>
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="7" fillId="5" fontId="12" numFmtId="0"/>
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="8" fillId="0" fontId="13" numFmtId="0"/>
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="9" fillId="0" fontId="14" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="6" fontId="15" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="7" fontId="16" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="8" fontId="17" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="9" fontId="18" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="10" fontId="19" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="11" fontId="19" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="12" fontId="18" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="13" fontId="18" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="14" fontId="19" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="15" fontId="19" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="16" fontId="18" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="17" fontId="18" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="18" fontId="19" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="19" fontId="19" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="20" fontId="18" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="21" fontId="18" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="22" fontId="19" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="23" fontId="19" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="24" fontId="18" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="25" fontId="18" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="26" fontId="19" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="27" fontId="19" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="28" fontId="18" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="29" fontId="18" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="30" fontId="19" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="31" fontId="19" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="32" fontId="18" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="20" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
+    <cellStyle builtinId="30" name="20% - Accent1" xfId="25"/>
+    <cellStyle builtinId="34" name="20% - Accent2" xfId="29"/>
+    <cellStyle builtinId="38" name="20% - Accent3" xfId="33"/>
+    <cellStyle builtinId="42" name="20% - Accent4" xfId="37"/>
+    <cellStyle builtinId="46" name="20% - Accent5" xfId="41"/>
+    <cellStyle builtinId="50" name="20% - Accent6" xfId="45"/>
+    <cellStyle builtinId="31" name="40% - Accent1" xfId="26"/>
+    <cellStyle builtinId="35" name="40% - Accent2" xfId="30"/>
+    <cellStyle builtinId="39" name="40% - Accent3" xfId="34"/>
+    <cellStyle builtinId="43" name="40% - Accent4" xfId="38"/>
+    <cellStyle builtinId="47" name="40% - Accent5" xfId="42"/>
+    <cellStyle builtinId="51" name="40% - Accent6" xfId="46"/>
+    <cellStyle builtinId="32" name="60% - Accent1" xfId="27"/>
+    <cellStyle builtinId="36" name="60% - Accent2" xfId="31"/>
+    <cellStyle builtinId="40" name="60% - Accent3" xfId="35"/>
+    <cellStyle builtinId="44" name="60% - Accent4" xfId="39"/>
+    <cellStyle builtinId="48" name="60% - Accent5" xfId="43"/>
+    <cellStyle builtinId="52" name="60% - Accent6" xfId="47"/>
+    <cellStyle builtinId="29" name="Accent1" xfId="24"/>
+    <cellStyle builtinId="33" name="Accent2" xfId="28"/>
+    <cellStyle builtinId="37" name="Accent3" xfId="32"/>
+    <cellStyle builtinId="41" name="Accent4" xfId="36"/>
+    <cellStyle builtinId="45" name="Accent5" xfId="40"/>
+    <cellStyle builtinId="49" name="Accent6" xfId="44"/>
+    <cellStyle builtinId="27" name="Bad" xfId="22"/>
+    <cellStyle builtinId="22" name="Calculation" xfId="17"/>
+    <cellStyle builtinId="23" name="Check Cell" xfId="18"/>
+    <cellStyle builtinId="3" name="Comma" xfId="1"/>
+    <cellStyle builtinId="6" name="Comma [0]" xfId="4"/>
+    <cellStyle builtinId="4" name="Currency" xfId="2"/>
+    <cellStyle builtinId="7" name="Currency [0]" xfId="5"/>
+    <cellStyle builtinId="53" name="Explanatory Text" xfId="48"/>
+    <cellStyle builtinId="9" name="Followed Hyperlink" xfId="7"/>
+    <cellStyle builtinId="26" name="Good" xfId="21"/>
+    <cellStyle builtinId="16" name="Heading 1" xfId="11"/>
+    <cellStyle builtinId="17" name="Heading 2" xfId="12"/>
+    <cellStyle builtinId="18" name="Heading 3" xfId="13"/>
+    <cellStyle builtinId="19" name="Heading 4" xfId="14"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="6"/>
+    <cellStyle builtinId="20" name="Input" xfId="15"/>
+    <cellStyle builtinId="24" name="Linked Cell" xfId="19"/>
+    <cellStyle builtinId="28" name="Neutral" xfId="23"/>
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle builtinId="10" name="Note" xfId="8"/>
+    <cellStyle builtinId="21" name="Output" xfId="16"/>
+    <cellStyle builtinId="5" name="Percent" xfId="3"/>
+    <cellStyle builtinId="15" name="Title" xfId="10"/>
+    <cellStyle builtinId="25" name="Total" xfId="20"/>
+    <cellStyle builtinId="11" name="Warning Text" xfId="9"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
       <font>
         <b/>
-        <i val="0"/>
+        <color rgb="FF000000"/>
       </font>
       <fill>
         <patternFill>
@@ -205,30 +882,21 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
+        <color rgb="FF000000"/>
       </font>
       <fill>
-        <patternFill patternType="none">
-          <bgColor indexed="65"/>
+        <patternFill>
+          <bgColor rgb="FFFFFFFF"/>
         </patternFill>
       </fill>
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2">
-    <tableStyle count="2" name="MySqlDefault" pivot="0" table="0">
+    <tableStyle count="2" name="MySqlDefault" pivot="0">
       <tableStyleElement dxfId="1" type="wholeTable"/>
       <tableStyleElement dxfId="0" type="headerRow"/>
     </tableStyle>
   </tableStyles>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -494,437 +1162,354 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.000000"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" width="5.25500011" collapsed="true" outlineLevel="0"/>
+    <col min="2" max="2" customWidth="true" width="17.12999916" collapsed="true" outlineLevel="0"/>
+    <col min="3" max="3" customWidth="true" width="16.75499916" collapsed="true" outlineLevel="0"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row ht="16.500000" r="1" spans="1:3">
+      <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row ht="16.500000" r="2" spans="1:3">
+      <c r="A2" s="0">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="B2" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="0">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+    </row>
+    <row ht="16.500000" r="3" spans="1:3">
+      <c r="A3" s="0">
+        <v>4</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="0">
         <v>2</v>
       </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
+    </row>
+    <row ht="16.500000" r="4" spans="1:3">
+      <c r="A4" s="0">
+        <v>7</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="0">
         <v>3</v>
       </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10">
-        <v>3</v>
-      </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins bottom="0.75" footer="0.30" header="0.30" left="0.70" right="0.70" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr customHeight="1" defaultRowHeight="15.000000"/>
+  <cols>
+    <col min="4" max="4" customWidth="true" width="12.63000011" collapsed="true" outlineLevel="0"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row ht="16.500000" r="1" spans="1:4">
+      <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="B1" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="0" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row ht="16.500000" r="2" spans="1:4">
+      <c r="A2" s="0">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="0">
         <v>100</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="0">
         <v>500</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row ht="16.500000" r="3" spans="1:4">
+      <c r="A3" s="0">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="0">
         <v>80</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="0">
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4">
-        <v>50</v>
-      </c>
-      <c r="D4">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5">
-        <v>20</v>
-      </c>
-      <c r="D5">
-        <v>10</v>
-      </c>
-    </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="0"/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins bottom="0.75" footer="0.30" header="0.30" left="0.70" right="0.70" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A4" sqref="A4:XFD5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.000000"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row ht="16.500000" r="1" spans="1:1">
+      <c r="A1" s="0" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row ht="16.500000" r="2" spans="1:1">
+      <c r="A2" s="0" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row ht="16.500000" r="3" spans="1:1">
+      <c r="A3" s="0" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>25</v>
-      </c>
-    </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins bottom="0.75" footer="0.30" header="0.30" left="0.70" right="0.70" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr customHeight="1" defaultRowHeight="15.000000"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="18.42578125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="33.85546875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="33.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.37999916" collapsed="true" outlineLevel="0"/>
+    <col min="4" max="4" customWidth="true" width="33.88000107" collapsed="true" outlineLevel="0"/>
+    <col min="5" max="5" customWidth="true" width="33.13000107" collapsed="true" outlineLevel="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row ht="16.500000" r="1" spans="1:5">
       <c r="A1" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2">
+        <v>67</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row ht="16.500000" r="2" spans="1:5">
+      <c r="A2" s="0">
         <v>0</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="0">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="0" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row ht="16.500000" r="3" spans="1:5">
+      <c r="A3" s="0">
         <v>1</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="0">
         <v>4</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="0" t="s">
         <v>32</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.25" r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row ht="16.500000" r="4" spans="1:5">
+      <c r="A4" s="0">
         <v>2</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="0">
         <v>7</v>
       </c>
-      <c r="C4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="C4" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="D4" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="0" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>73</v>
       </c>
       <c r="B5" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="C5" t="s">
         <v>22</v>
       </c>
       <c r="D5" t="s">
-        <v>35</v>
+        <v>96</v>
       </c>
       <c r="E5" t="s">
-        <v>36</v>
+        <v>97</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>33</v>
+        <v>73</v>
       </c>
       <c r="B6" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="C6" t="s">
         <v>22</v>
       </c>
       <c r="D6" t="s">
-        <v>35</v>
+        <v>98</v>
       </c>
       <c r="E6" t="s">
-        <v>36</v>
+        <v>99</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>33</v>
+        <v>73</v>
       </c>
       <c r="B7" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="C7" t="s">
         <v>22</v>
       </c>
       <c r="D7" t="s">
-        <v>35</v>
+        <v>98</v>
       </c>
       <c r="E7" t="s">
-        <v>36</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="0"/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins bottom="0.75" footer="0.30" header="0.30" left="0.70" right="0.70" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O61" sqref="O61"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr customHeight="1" defaultRowHeight="15.000000"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="16.13000011" collapsed="true" outlineLevel="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row ht="16.500000" r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="B1" s="0" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row ht="16.500000" r="2" spans="1:2">
+      <c r="A2" s="0">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="0" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row ht="16.500000" r="3" spans="1:2">
+      <c r="A3" s="0">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="0" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row ht="16.500000" r="4" spans="1:2">
+      <c r="A4" s="0">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="0" t="s">
         <v>15</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="0"/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins bottom="0.75" footer="0.30" header="0.30" left="0.70" right="0.70" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Close #50 - Loan creation log implementation
- LoanLogDAO implementation
- General tests updated
- Entities modified
</commit_message>
<xml_diff>
--- a/core/excel/Test.xlsx
+++ b/core/excel/Test.xlsx
@@ -4,21 +4,23 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="3" windowHeight="11595" windowWidth="25755" xWindow="360" yWindow="30"/>
+    <workbookView activeTab="4" windowHeight="11595" windowWidth="25755" xWindow="360" yWindow="30"/>
   </bookViews>
   <sheets>
     <sheet name="Tools" r:id="rId1" sheetId="1"/>
     <sheet name="Supplies" r:id="rId2" sheetId="3"/>
     <sheet name="Borrowers" r:id="rId3" sheetId="4"/>
     <sheet name="Loans" r:id="rId4" sheetId="5"/>
-    <sheet name="TipoHerramienta" r:id="rId5" sheetId="2"/>
+    <sheet name="PrestamosLog" r:id="rId5" sheetId="6"/>
+    <sheet name="RetirosLog" r:id="rId6" sheetId="7"/>
+    <sheet name="TipoHerramienta" r:id="rId7" sheetId="2"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="186">
   <si>
     <t>ID</t>
   </si>
@@ -239,85 +241,343 @@
     <t>Nombre</t>
   </si>
   <si>
+    <t>Tue May 29 13:50:33 ART 2018</t>
+  </si>
+  <si>
+    <t>Wed May 30 13:50:33 ART 2018</t>
+  </si>
+  <si>
     <t>0</t>
   </si>
   <si>
-    <t>Tue May 29 14:01:15 ART 2018</t>
-  </si>
-  <si>
-    <t>Wed May 30 14:01:15 ART 2018</t>
-  </si>
-  <si>
-    <t>Tue May 29 14:01:16 ART 2018</t>
-  </si>
-  <si>
-    <t>Wed May 30 14:01:16 ART 2018</t>
-  </si>
-  <si>
-    <t>Tue May 29 14:03:03 ART 2018</t>
-  </si>
-  <si>
-    <t>Wed May 30 14:03:03 ART 2018</t>
-  </si>
-  <si>
-    <t>Tue May 29 14:03:04 ART 2018</t>
-  </si>
-  <si>
-    <t>Wed May 30 14:03:04 ART 2018</t>
-  </si>
-  <si>
-    <t>Tue May 29 15:53:51 ART 2018</t>
-  </si>
-  <si>
-    <t>Wed May 30 15:53:51 ART 2018</t>
-  </si>
-  <si>
-    <t>Tue May 29 15:53:52 ART 2018</t>
-  </si>
-  <si>
-    <t>Wed May 30 15:53:52 ART 2018</t>
-  </si>
-  <si>
-    <t>Tue May 29 15:53:53 ART 2018</t>
-  </si>
-  <si>
-    <t>Wed May 30 15:53:53 ART 2018</t>
-  </si>
-  <si>
-    <t>Tue May 29 16:02:11 ART 2018</t>
-  </si>
-  <si>
-    <t>Wed May 30 16:02:11 ART 2018</t>
-  </si>
-  <si>
-    <t>Tue May 29 16:02:12 ART 2018</t>
-  </si>
-  <si>
-    <t>Wed May 30 16:02:12 ART 2018</t>
-  </si>
-  <si>
-    <t>Tue May 29 16:03:08 ART 2018</t>
-  </si>
-  <si>
-    <t>Wed May 30 16:03:08 ART 2018</t>
-  </si>
-  <si>
-    <t>Tue May 29 16:03:09 ART 2018</t>
-  </si>
-  <si>
-    <t>Wed May 30 16:03:09 ART 2018</t>
-  </si>
-  <si>
-    <t>Tue May 29 17:01:50 ART 2018</t>
-  </si>
-  <si>
-    <t>Wed May 30 17:01:50 ART 2018</t>
-  </si>
-  <si>
-    <t>Tue May 29 17:01:51 ART 2018</t>
-  </si>
-  <si>
-    <t>Wed May 30 17:01:51 ART 2018</t>
+    <t>Tue May 29 15:31:57 ART 2018</t>
+  </si>
+  <si>
+    <t>Wed May 30 15:31:57 ART 2018</t>
+  </si>
+  <si>
+    <t>Tue May 29 15:32:02 ART 2018</t>
+  </si>
+  <si>
+    <t>Wed May 30 15:32:02 ART 2018</t>
+  </si>
+  <si>
+    <t>Tue May 29 15:33:01 ART 2018</t>
+  </si>
+  <si>
+    <t>Wed May 30 15:33:01 ART 2018</t>
+  </si>
+  <si>
+    <t>Tue May 29 15:52:19 ART 2018</t>
+  </si>
+  <si>
+    <t>Wed May 30 15:52:19 ART 2018</t>
+  </si>
+  <si>
+    <t>Tue May 29 15:53:14 ART 2018</t>
+  </si>
+  <si>
+    <t>Wed May 30 15:53:14 ART 2018</t>
+  </si>
+  <si>
+    <t>Tue May 29 15:57:56 ART 2018</t>
+  </si>
+  <si>
+    <t>Wed May 30 15:57:56 ART 2018</t>
+  </si>
+  <si>
+    <t>Tue May 29 15:58:39 ART 2018</t>
+  </si>
+  <si>
+    <t>Wed May 30 15:58:39 ART 2018</t>
+  </si>
+  <si>
+    <t>Tue May 29 15:58:44 ART 2018</t>
+  </si>
+  <si>
+    <t>Wed May 30 15:58:44 ART 2018</t>
+  </si>
+  <si>
+    <t>Tue May 29 15:59:21 ART 2018</t>
+  </si>
+  <si>
+    <t>Wed May 30 15:59:21 ART 2018</t>
+  </si>
+  <si>
+    <t>Tue May 29 16:04:44 ART 2018</t>
+  </si>
+  <si>
+    <t>Wed May 30 16:04:44 ART 2018</t>
+  </si>
+  <si>
+    <t>Elemento</t>
+  </si>
+  <si>
+    <t>Accion</t>
+  </si>
+  <si>
+    <t>Apertura</t>
+  </si>
+  <si>
+    <t>29-05</t>
+  </si>
+  <si>
+    <t>Cierre</t>
+  </si>
+  <si>
+    <t>30-05</t>
+  </si>
+  <si>
+    <t>Fecha creacion</t>
+  </si>
+  <si>
+    <t>Cantidad</t>
+  </si>
+  <si>
+    <t>13-09</t>
+  </si>
+  <si>
+    <t>Tue May 29 19:35:01 ART 2018</t>
+  </si>
+  <si>
+    <t>Tue May 29 19:53:41 ART 2018</t>
+  </si>
+  <si>
+    <t>Tue May 29 19:54:18 ART 2018</t>
+  </si>
+  <si>
+    <t>Tue May 29 19:54:51 ART 2018</t>
+  </si>
+  <si>
+    <t>Tue May 29 20:10:40 ART 2018</t>
+  </si>
+  <si>
+    <t>Tue May 29 22:03:29 ART 2018</t>
+  </si>
+  <si>
+    <t>Tue May 29 22:03:32 ART 2018</t>
+  </si>
+  <si>
+    <t>Tue May 29 22:04:57 ART 2018</t>
+  </si>
+  <si>
+    <t>Tue May 29 22:05:13 ART 2018</t>
+  </si>
+  <si>
+    <t>Tue May 29 22:05:17 ART 2018</t>
+  </si>
+  <si>
+    <t>Taladro #2</t>
+  </si>
+  <si>
+    <t>Destornillador #2</t>
+  </si>
+  <si>
+    <t>Tue May 29 22:14:27 ART 2018</t>
+  </si>
+  <si>
+    <t>Tue May 29 22:16:30 ART 2018</t>
+  </si>
+  <si>
+    <t>Tue May 29 22:20:20 ART 2018</t>
+  </si>
+  <si>
+    <t>Tue May 29 22:20:24 ART 2018</t>
+  </si>
+  <si>
+    <t>Tue May 29 22:28:13 ART 2018</t>
+  </si>
+  <si>
+    <t>Tue May 29 22:28:16 ART 2018</t>
+  </si>
+  <si>
+    <t>Tue May 29 23:22:00 ART 2018</t>
+  </si>
+  <si>
+    <t>Martillo</t>
+  </si>
+  <si>
+    <t>Tue May 29 23:22:01 ART 2018</t>
+  </si>
+  <si>
+    <t>Tue May 29 23:22:02 ART 2018</t>
+  </si>
+  <si>
+    <t>Taladro #`</t>
+  </si>
+  <si>
+    <t>Taladro #1</t>
+  </si>
+  <si>
+    <t>Wed May 30 00:25:33 ART 2018</t>
+  </si>
+  <si>
+    <t>Martillo #30</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>Wed May 30 00:32:19 ART 2018</t>
+  </si>
+  <si>
+    <t>Wed May 30 00:34:19 ART 2018</t>
+  </si>
+  <si>
+    <t>Wed May 30 00:45:11 ART 2018</t>
+  </si>
+  <si>
+    <t>Wed May 30 00:45:12 ART 2018</t>
+  </si>
+  <si>
+    <t>Wed May 30 00:45:15 ART 2018</t>
+  </si>
+  <si>
+    <t>Wed May 30 00:45:16 ART 2018</t>
+  </si>
+  <si>
+    <t>Wed May 30 00:45:19 ART 2018</t>
+  </si>
+  <si>
+    <t>Wed May 30 00:45:20 ART 2018</t>
+  </si>
+  <si>
+    <t>Wed May 30 00:45:22 ART 2018</t>
+  </si>
+  <si>
+    <t>Wed May 30 00:45:23 ART 2018</t>
+  </si>
+  <si>
+    <t>Wed May 30 00:48:34 ART 2018</t>
+  </si>
+  <si>
+    <t>Wed May 30 00:48:35 ART 2018</t>
+  </si>
+  <si>
+    <t>Wed May 30 00:52:01 ART 2018</t>
+  </si>
+  <si>
+    <t>Wed May 30 00:52:02 ART 2018</t>
+  </si>
+  <si>
+    <t>Wed May 30 00:52:24 ART 2018</t>
+  </si>
+  <si>
+    <t>Wed May 30 00:52:25 ART 2018</t>
+  </si>
+  <si>
+    <t>Wed May 30 00:52:40 ART 2018</t>
+  </si>
+  <si>
+    <t>Wed May 30 00:52:41 ART 2018</t>
+  </si>
+  <si>
+    <t>Wed May 30 00:52:51 ART 2018</t>
+  </si>
+  <si>
+    <t>Wed May 30 00:52:52 ART 2018</t>
+  </si>
+  <si>
+    <t>Wed May 30 16:46:40 ART 2018</t>
+  </si>
+  <si>
+    <t>Wed May 30 16:46:41 ART 2018</t>
+  </si>
+  <si>
+    <t>Wed May 30 16:46:44 ART 2018</t>
+  </si>
+  <si>
+    <t>Wed May 30 16:46:45 ART 2018</t>
+  </si>
+  <si>
+    <t>Wed May 30 16:47:04 ART 2018</t>
+  </si>
+  <si>
+    <t>Wed May 30 16:48:15 ART 2018</t>
+  </si>
+  <si>
+    <t>Wed May 30 16:48:16 ART 2018</t>
+  </si>
+  <si>
+    <t>Wed May 30 16:48:55 ART 2018</t>
+  </si>
+  <si>
+    <t>Wed May 30 16:48:56 ART 2018</t>
+  </si>
+  <si>
+    <t>Wed May 30 16:48:59 ART 2018</t>
+  </si>
+  <si>
+    <t>Wed May 30 16:49:00 ART 2018</t>
+  </si>
+  <si>
+    <t>Wed May 30 17:02:33 ART 2018</t>
+  </si>
+  <si>
+    <t>Wed May 30 17:02:34 ART 2018</t>
+  </si>
+  <si>
+    <t>Wed May 30 17:03:28 ART 2018</t>
+  </si>
+  <si>
+    <t>Wed May 30 17:03:29 ART 2018</t>
+  </si>
+  <si>
+    <t>Wed May 30 17:07:07 ART 2018</t>
+  </si>
+  <si>
+    <t>Wed May 30 17:07:08 ART 2018</t>
+  </si>
+  <si>
+    <t>Wed May 30 17:07:09 ART 2018</t>
+  </si>
+  <si>
+    <t>Wed May 30 17:09:26 ART 2018</t>
+  </si>
+  <si>
+    <t>Wed May 30 17:09:27 ART 2018</t>
+  </si>
+  <si>
+    <t>Wed May 30 20:10:27 ART 2018</t>
+  </si>
+  <si>
+    <t>Wed May 30 20:10:28 ART 2018</t>
+  </si>
+  <si>
+    <t>Wed May 30 20:10:29 ART 2018</t>
+  </si>
+  <si>
+    <t>Thu May 31 22:27:18 ART 2018</t>
+  </si>
+  <si>
+    <t>Thu May 31 22:27:19 ART 2018</t>
+  </si>
+  <si>
+    <t>Thu May 31 22:27:20 ART 2018</t>
+  </si>
+  <si>
+    <t>Thu May 31 22:30:04 ART 2018</t>
+  </si>
+  <si>
+    <t>Thu May 31 22:30:05 ART 2018</t>
+  </si>
+  <si>
+    <t>Thu May 31 22:30:06 ART 2018</t>
+  </si>
+  <si>
+    <t>Thu May 31 22:30:07 ART 2018</t>
+  </si>
+  <si>
+    <t>Thu May 31 22:31:34 ART 2018</t>
+  </si>
+  <si>
+    <t>Thu May 31 22:31:35 ART 2018</t>
+  </si>
+  <si>
+    <t>Thu May 31 22:31:36 ART 2018</t>
+  </si>
+  <si>
+    <t>Thu May 31 22:31:37 ART 2018</t>
   </si>
 </sst>
 </file>
@@ -1163,10 +1423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView workbookViewId="0" zoomScale="400">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.000000"/>
@@ -1220,6 +1480,28 @@
         <v>3</v>
       </c>
     </row>
+    <row ht="16.500000" r="5" spans="1:3">
+      <c r="A5" s="0">
+        <v>2</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="C5" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row ht="16.500000" r="6" spans="1:3">
+      <c r="A6" s="0">
+        <v>3</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="C6" s="0">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins bottom="0.75" footer="0.30" header="0.30" left="0.70" right="0.70" top="0.75"/>
@@ -1231,8 +1513,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView workbookViewId="0" zoomScale="399">
+      <selection activeCell="C1" sqref="C1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultRowHeight="15.000000"/>
@@ -1293,11 +1575,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView workbookViewId="0" zoomScale="400">
       <selection activeCell="A4" sqref="A4:XFD5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.000000"/>
+  <sheetFormatPr customHeight="1" defaultRowHeight="15.000000"/>
   <sheetData>
     <row ht="16.500000" r="1" spans="1:1">
       <c r="A1" s="0" t="s">
@@ -1323,20 +1605,19 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView workbookViewId="0" zoomScale="356">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultRowHeight="15.000000"/>
   <cols>
     <col min="2" max="2" customWidth="true" width="18.37999916" collapsed="true" outlineLevel="0"/>
     <col min="4" max="4" customWidth="true" width="33.88000107" collapsed="true" outlineLevel="0"/>
-    <col min="5" max="5" customWidth="true" width="33.13000107" collapsed="true" outlineLevel="0"/>
   </cols>
   <sheetData>
-    <row ht="16.500000" r="1" spans="1:5">
+    <row ht="16.500000" r="1" spans="1:4">
       <c r="A1" s="2" t="s">
         <v>67</v>
       </c>
@@ -1349,11 +1630,8 @@
       <c r="D1" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="E1" s="0" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row ht="16.500000" r="2" spans="1:5">
+    </row>
+    <row ht="16.500000" r="2" spans="1:4">
       <c r="A2" s="0">
         <v>0</v>
       </c>
@@ -1366,11 +1644,8 @@
       <c r="D2" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="E2" s="0" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row ht="16.500000" r="3" spans="1:5">
+    </row>
+    <row ht="16.500000" r="3" spans="1:4">
       <c r="A3" s="0">
         <v>1</v>
       </c>
@@ -1383,11 +1658,8 @@
       <c r="D3" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="E3" s="0" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row ht="16.500000" r="4" spans="1:5">
+    </row>
+    <row ht="16.500000" r="4" spans="1:4">
       <c r="A4" s="0">
         <v>2</v>
       </c>
@@ -1399,60 +1671,6 @@
       </c>
       <c r="D4" s="0" t="s">
         <v>31</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>73</v>
-      </c>
-      <c r="B5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" t="s">
-        <v>96</v>
-      </c>
-      <c r="E5" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>73</v>
-      </c>
-      <c r="B6" t="s">
-        <v>47</v>
-      </c>
-      <c r="C6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" t="s">
-        <v>98</v>
-      </c>
-      <c r="E6" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s">
-        <v>73</v>
-      </c>
-      <c r="B7" t="s">
-        <v>47</v>
-      </c>
-      <c r="C7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" t="s">
-        <v>98</v>
-      </c>
-      <c r="E7" t="s">
-        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -1464,10 +1682,491 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0" zoomScale="385">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultRowHeight="16.500000"/>
+  <cols>
+    <col min="2" max="2" customWidth="true" width="14.25500011" collapsed="true" outlineLevel="0"/>
+    <col min="3" max="3" customWidth="true" width="10.63000011" collapsed="true" outlineLevel="0"/>
+    <col min="5" max="5" customWidth="true" width="31.25499916" collapsed="true" outlineLevel="0"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="0">
+        <v>0</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="0">
+        <v>1</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="0">
+        <v>2</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" t="s">
+        <v>98</v>
+      </c>
+      <c r="E5" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" t="s">
+        <v>115</v>
+      </c>
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" t="s">
+        <v>98</v>
+      </c>
+      <c r="E6" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" t="s">
+        <v>100</v>
+      </c>
+      <c r="E7" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" t="s">
+        <v>115</v>
+      </c>
+      <c r="C8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" t="s">
+        <v>98</v>
+      </c>
+      <c r="E8" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" t="s">
+        <v>115</v>
+      </c>
+      <c r="C9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" t="s">
+        <v>98</v>
+      </c>
+      <c r="E9" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" t="s">
+        <v>115</v>
+      </c>
+      <c r="C10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" t="s">
+        <v>98</v>
+      </c>
+      <c r="E10" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" t="s">
+        <v>115</v>
+      </c>
+      <c r="C11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" t="s">
+        <v>98</v>
+      </c>
+      <c r="E11" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" t="s">
+        <v>115</v>
+      </c>
+      <c r="C12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" t="s">
+        <v>98</v>
+      </c>
+      <c r="E12" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" t="s">
+        <v>115</v>
+      </c>
+      <c r="C13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" t="s">
+        <v>98</v>
+      </c>
+      <c r="E13" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" t="s">
+        <v>115</v>
+      </c>
+      <c r="C14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" t="s">
+        <v>100</v>
+      </c>
+      <c r="E14" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" t="s">
+        <v>115</v>
+      </c>
+      <c r="C15" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" t="s">
+        <v>98</v>
+      </c>
+      <c r="E15" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" t="s">
+        <v>115</v>
+      </c>
+      <c r="C16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" t="s">
+        <v>98</v>
+      </c>
+      <c r="E16" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" t="s">
+        <v>115</v>
+      </c>
+      <c r="C17" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" t="s">
+        <v>98</v>
+      </c>
+      <c r="E17" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" t="s">
+        <v>115</v>
+      </c>
+      <c r="C18" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" t="s">
+        <v>98</v>
+      </c>
+      <c r="E18" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" t="s">
+        <v>115</v>
+      </c>
+      <c r="C19" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" t="s">
+        <v>98</v>
+      </c>
+      <c r="E19" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" t="s">
+        <v>115</v>
+      </c>
+      <c r="C20" t="s">
+        <v>22</v>
+      </c>
+      <c r="D20" t="s">
+        <v>98</v>
+      </c>
+      <c r="E20" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" t="s">
+        <v>115</v>
+      </c>
+      <c r="C21" t="s">
+        <v>22</v>
+      </c>
+      <c r="D21" t="s">
+        <v>100</v>
+      </c>
+      <c r="E21" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" t="s">
+        <v>115</v>
+      </c>
+      <c r="C22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D22" t="s">
+        <v>98</v>
+      </c>
+      <c r="E22" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>33</v>
+      </c>
+      <c r="B23" t="s">
+        <v>115</v>
+      </c>
+      <c r="C23" t="s">
+        <v>22</v>
+      </c>
+      <c r="D23" t="s">
+        <v>98</v>
+      </c>
+      <c r="E23" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>33</v>
+      </c>
+      <c r="B24" t="s">
+        <v>115</v>
+      </c>
+      <c r="C24" t="s">
+        <v>22</v>
+      </c>
+      <c r="D24" t="s">
+        <v>98</v>
+      </c>
+      <c r="E24" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>33</v>
+      </c>
+      <c r="B25" t="s">
+        <v>115</v>
+      </c>
+      <c r="C25" t="s">
+        <v>22</v>
+      </c>
+      <c r="D25" t="s">
+        <v>98</v>
+      </c>
+      <c r="E25" t="s">
+        <v>185</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins bottom="0.75" footer="0.30" header="0.30" left="0.70" right="0.70" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="400">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultRowHeight="16.500000"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" width="8.00500011" collapsed="true" outlineLevel="0"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins bottom="0.75" footer="0.30" header="0.30" left="0.70" right="0.70" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O61" sqref="O61"/>
+    <sheetView workbookViewId="0" zoomScale="400">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultRowHeight="15.000000"/>

</xml_diff>

<commit_message>
Close #54 - Error system implementation
- ErrorSystem, ErrorNotification & ExcelVerified added
- General tests implementation added
</commit_message>
<xml_diff>
--- a/core/excel/Test.xlsx
+++ b/core/excel/Test.xlsx
@@ -4,24 +4,23 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="30" windowWidth="25755" windowHeight="11595" activeTab="5"/>
+    <workbookView activeTab="5" windowHeight="11595" windowWidth="25755" xWindow="360" yWindow="30"/>
   </bookViews>
   <sheets>
-    <sheet name="Tools" sheetId="1" r:id="rId1"/>
-    <sheet name="Supplies" sheetId="3" r:id="rId2"/>
-    <sheet name="Borrowers" sheetId="4" r:id="rId3"/>
-    <sheet name="Loans" sheetId="5" r:id="rId4"/>
-    <sheet name="PrestamosLog" sheetId="6" r:id="rId5"/>
-    <sheet name="RetirosLog" sheetId="7" r:id="rId6"/>
-    <sheet name="TipoHerramienta" sheetId="2" r:id="rId7"/>
+    <sheet name="Tools" r:id="rId1" sheetId="1"/>
+    <sheet name="Supplies" r:id="rId2" sheetId="3"/>
+    <sheet name="Borrowers" r:id="rId3" sheetId="4"/>
+    <sheet name="Loans" r:id="rId4" sheetId="5"/>
+    <sheet name="PrestamosLog" r:id="rId5" sheetId="6"/>
+    <sheet name="RetirosLog" r:id="rId6" sheetId="7"/>
+    <sheet name="TipoHerramienta" r:id="rId7" sheetId="2"/>
   </sheets>
-  <definedNames/>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="204">
   <si>
     <t>ID</t>
   </si>
@@ -582,6 +581,57 @@
   </si>
   <si>
     <t>Thu May 31 22:46:03 ART 2018</t>
+  </si>
+  <si>
+    <t>Fri Jun 01 03:27:00 ART 2018</t>
+  </si>
+  <si>
+    <t>Fri Jun 01 03:27:02 ART 2018</t>
+  </si>
+  <si>
+    <t>Fri Jun 01 03:27:03 ART 2018</t>
+  </si>
+  <si>
+    <t>Fri Jun 01 03:27:04 ART 2018</t>
+  </si>
+  <si>
+    <t>Fri Jun 01 03:27:05 ART 2018</t>
+  </si>
+  <si>
+    <t>Fri Jun 01 15:13:50 ART 2018</t>
+  </si>
+  <si>
+    <t>Fri Jun 01 18:00:41 ART 2018</t>
+  </si>
+  <si>
+    <t>Fri Jun 01 18:00:43 ART 2018</t>
+  </si>
+  <si>
+    <t>Fri Jun 01 18:00:44 ART 2018</t>
+  </si>
+  <si>
+    <t>Fri Jun 01 18:00:45 ART 2018</t>
+  </si>
+  <si>
+    <t>Fri Jun 01 18:00:46 ART 2018</t>
+  </si>
+  <si>
+    <t>Fri Jun 01 18:01:21 ART 2018</t>
+  </si>
+  <si>
+    <t>Fri Jun 01 18:01:23 ART 2018</t>
+  </si>
+  <si>
+    <t>Fri Jun 01 18:01:24 ART 2018</t>
+  </si>
+  <si>
+    <t>Fri Jun 01 18:01:25 ART 2018</t>
+  </si>
+  <si>
+    <t>Fri Jun 01 18:01:26 ART 2018</t>
+  </si>
+  <si>
+    <t>Fri Jun 01 18:01:27 ART 2018</t>
   </si>
 </sst>
 </file>
@@ -1026,111 +1076,111 @@
     </border>
   </borders>
   <cellStyleXfs count="49">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0"/>
-    <xf numFmtId="7" fontId="0" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0"/>
-    <xf numFmtId="5" fontId="0" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyAlignment="0" applyFont="0" applyNumberFormat="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="5" applyAlignment="0" applyNumberFormat="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="6" applyAlignment="0" applyNumberFormat="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyAlignment="0" applyNumberFormat="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="7" applyAlignment="0" applyNumberFormat="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="43"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="7"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="9"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="41"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="5"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf applyAlignment="0" applyFont="0" applyNumberFormat="0" applyProtection="0" borderId="1" fillId="2" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="4" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="5" numFmtId="0"/>
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="2" fillId="0" fontId="6" numFmtId="0"/>
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="3" fillId="0" fontId="7" numFmtId="0"/>
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="4" fillId="0" fontId="8" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="8" numFmtId="0"/>
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="5" fillId="3" fontId="9" numFmtId="0"/>
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="6" fillId="4" fontId="10" numFmtId="0"/>
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="5" fillId="4" fontId="11" numFmtId="0"/>
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="7" fillId="5" fontId="12" numFmtId="0"/>
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="8" fillId="0" fontId="13" numFmtId="0"/>
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="9" fillId="0" fontId="14" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="6" fontId="15" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="7" fontId="16" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="8" fontId="17" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="9" fontId="18" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="10" fontId="19" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="11" fontId="19" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="12" fontId="18" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="13" fontId="18" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="14" fontId="19" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="15" fontId="19" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="16" fontId="18" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="17" fontId="18" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="18" fontId="19" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="19" fontId="19" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="20" fontId="18" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="21" fontId="18" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="22" fontId="19" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="23" fontId="19" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="24" fontId="18" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="25" fontId="18" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="26" fontId="19" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="27" fontId="19" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="28" fontId="18" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="29" fontId="18" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="30" fontId="19" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="31" fontId="19" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="32" fontId="18" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="20" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="49">
-    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
-    <cellStyle name="20% - Accent2" xfId="29" builtinId="34"/>
-    <cellStyle name="20% - Accent3" xfId="33" builtinId="38"/>
-    <cellStyle name="20% - Accent4" xfId="37" builtinId="42"/>
-    <cellStyle name="20% - Accent5" xfId="41" builtinId="46"/>
-    <cellStyle name="20% - Accent6" xfId="45" builtinId="50"/>
-    <cellStyle name="40% - Accent1" xfId="26" builtinId="31"/>
-    <cellStyle name="40% - Accent2" xfId="30" builtinId="35"/>
-    <cellStyle name="40% - Accent3" xfId="34" builtinId="39"/>
-    <cellStyle name="40% - Accent4" xfId="38" builtinId="43"/>
-    <cellStyle name="40% - Accent5" xfId="42" builtinId="47"/>
-    <cellStyle name="40% - Accent6" xfId="46" builtinId="51"/>
-    <cellStyle name="60% - Accent1" xfId="27" builtinId="32"/>
-    <cellStyle name="60% - Accent2" xfId="31" builtinId="36"/>
-    <cellStyle name="60% - Accent3" xfId="35" builtinId="40"/>
-    <cellStyle name="60% - Accent4" xfId="39" builtinId="44"/>
-    <cellStyle name="60% - Accent5" xfId="43" builtinId="48"/>
-    <cellStyle name="60% - Accent6" xfId="47" builtinId="52"/>
-    <cellStyle name="Accent1" xfId="24" builtinId="29"/>
-    <cellStyle name="Accent2" xfId="28" builtinId="33"/>
-    <cellStyle name="Accent3" xfId="32" builtinId="37"/>
-    <cellStyle name="Accent4" xfId="36" builtinId="41"/>
-    <cellStyle name="Accent5" xfId="40" builtinId="45"/>
-    <cellStyle name="Accent6" xfId="44" builtinId="49"/>
-    <cellStyle name="Bad" xfId="22" builtinId="27"/>
-    <cellStyle name="Calculation" xfId="17" builtinId="22"/>
-    <cellStyle name="Check Cell" xfId="18" builtinId="23"/>
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
-    <cellStyle name="Currency" xfId="2" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
-    <cellStyle name="Explanatory Text" xfId="48" builtinId="53"/>
-    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
-    <cellStyle name="Good" xfId="21" builtinId="26"/>
-    <cellStyle name="Heading 1" xfId="11" builtinId="16"/>
-    <cellStyle name="Heading 2" xfId="12" builtinId="17"/>
-    <cellStyle name="Heading 3" xfId="13" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="14" builtinId="19"/>
-    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
-    <cellStyle name="Input" xfId="15" builtinId="20"/>
-    <cellStyle name="Linked Cell" xfId="19" builtinId="24"/>
-    <cellStyle name="Neutral" xfId="23" builtinId="28"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="8" builtinId="10"/>
-    <cellStyle name="Output" xfId="16" builtinId="21"/>
-    <cellStyle name="Percent" xfId="3" builtinId="5"/>
-    <cellStyle name="Title" xfId="10" builtinId="15"/>
-    <cellStyle name="Total" xfId="20" builtinId="25"/>
-    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
+    <cellStyle builtinId="30" name="20% - Accent1" xfId="25"/>
+    <cellStyle builtinId="34" name="20% - Accent2" xfId="29"/>
+    <cellStyle builtinId="38" name="20% - Accent3" xfId="33"/>
+    <cellStyle builtinId="42" name="20% - Accent4" xfId="37"/>
+    <cellStyle builtinId="46" name="20% - Accent5" xfId="41"/>
+    <cellStyle builtinId="50" name="20% - Accent6" xfId="45"/>
+    <cellStyle builtinId="31" name="40% - Accent1" xfId="26"/>
+    <cellStyle builtinId="35" name="40% - Accent2" xfId="30"/>
+    <cellStyle builtinId="39" name="40% - Accent3" xfId="34"/>
+    <cellStyle builtinId="43" name="40% - Accent4" xfId="38"/>
+    <cellStyle builtinId="47" name="40% - Accent5" xfId="42"/>
+    <cellStyle builtinId="51" name="40% - Accent6" xfId="46"/>
+    <cellStyle builtinId="32" name="60% - Accent1" xfId="27"/>
+    <cellStyle builtinId="36" name="60% - Accent2" xfId="31"/>
+    <cellStyle builtinId="40" name="60% - Accent3" xfId="35"/>
+    <cellStyle builtinId="44" name="60% - Accent4" xfId="39"/>
+    <cellStyle builtinId="48" name="60% - Accent5" xfId="43"/>
+    <cellStyle builtinId="52" name="60% - Accent6" xfId="47"/>
+    <cellStyle builtinId="29" name="Accent1" xfId="24"/>
+    <cellStyle builtinId="33" name="Accent2" xfId="28"/>
+    <cellStyle builtinId="37" name="Accent3" xfId="32"/>
+    <cellStyle builtinId="41" name="Accent4" xfId="36"/>
+    <cellStyle builtinId="45" name="Accent5" xfId="40"/>
+    <cellStyle builtinId="49" name="Accent6" xfId="44"/>
+    <cellStyle builtinId="27" name="Bad" xfId="22"/>
+    <cellStyle builtinId="22" name="Calculation" xfId="17"/>
+    <cellStyle builtinId="23" name="Check Cell" xfId="18"/>
+    <cellStyle builtinId="3" name="Comma" xfId="1"/>
+    <cellStyle builtinId="6" name="Comma [0]" xfId="4"/>
+    <cellStyle builtinId="4" name="Currency" xfId="2"/>
+    <cellStyle builtinId="7" name="Currency [0]" xfId="5"/>
+    <cellStyle builtinId="53" name="Explanatory Text" xfId="48"/>
+    <cellStyle builtinId="9" name="Followed Hyperlink" xfId="7"/>
+    <cellStyle builtinId="26" name="Good" xfId="21"/>
+    <cellStyle builtinId="16" name="Heading 1" xfId="11"/>
+    <cellStyle builtinId="17" name="Heading 2" xfId="12"/>
+    <cellStyle builtinId="18" name="Heading 3" xfId="13"/>
+    <cellStyle builtinId="19" name="Heading 4" xfId="14"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="6"/>
+    <cellStyle builtinId="20" name="Input" xfId="15"/>
+    <cellStyle builtinId="24" name="Linked Cell" xfId="19"/>
+    <cellStyle builtinId="28" name="Neutral" xfId="23"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle builtinId="10" name="Note" xfId="8"/>
+    <cellStyle builtinId="21" name="Output" xfId="16"/>
+    <cellStyle builtinId="5" name="Percent" xfId="3"/>
+    <cellStyle builtinId="15" name="Title" xfId="10"/>
+    <cellStyle builtinId="25" name="Total" xfId="20"/>
+    <cellStyle builtinId="11" name="Warning Text" xfId="9"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -1155,10 +1205,10 @@
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" count="2">
-      <tableStyleElement type="wholeTable" dxfId="1"/>
-      <tableStyleElement type="headerRow" dxfId="0"/>
+  <tableStyles count="1" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2">
+    <tableStyle count="2" name="MySqlDefault" pivot="0">
+      <tableStyleElement dxfId="1" type="wholeTable"/>
+      <tableStyleElement dxfId="0" type="headerRow"/>
     </tableStyle>
   </tableStyles>
 </styleSheet>
@@ -1427,20 +1477,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView zoomScale="400" workbookViewId="0">
+    <sheetView workbookViewId="0" zoomScale="400">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.000000"/>
   <cols>
-    <col min="1" max="1" width="5.25500011" customWidth="1" outlineLevel="0"/>
-    <col min="2" max="2" width="17.12999916" customWidth="1" outlineLevel="0"/>
-    <col min="3" max="3" width="16.75499916" customWidth="1" outlineLevel="0"/>
+    <col min="1" max="1" customWidth="true" width="5.25500011" collapsed="true" outlineLevel="0"/>
+    <col min="2" max="2" customWidth="true" width="17.12999916" collapsed="true" outlineLevel="0"/>
+    <col min="3" max="3" customWidth="true" width="16.75499916" collapsed="true" outlineLevel="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16.500000">
+    <row ht="16.500000" r="1" spans="1:3">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
@@ -1451,7 +1501,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="16.500000">
+    <row ht="16.500000" r="2" spans="1:3">
       <c r="A2" s="0">
         <v>1</v>
       </c>
@@ -1462,7 +1512,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="16.500000">
+    <row ht="16.500000" r="3" spans="1:3">
       <c r="A3" s="0">
         <v>4</v>
       </c>
@@ -1473,7 +1523,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="16.500000">
+    <row ht="16.500000" r="4" spans="1:3">
       <c r="A4" s="0">
         <v>7</v>
       </c>
@@ -1484,7 +1534,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="16.500000">
+    <row ht="16.500000" r="5" spans="1:3">
       <c r="A5" s="0">
         <v>2</v>
       </c>
@@ -1495,7 +1545,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="16.500000">
+    <row ht="16.500000" r="6" spans="1:3">
       <c r="A6" s="0">
         <v>3</v>
       </c>
@@ -1508,25 +1558,25 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.70" right="0.70" top="0.75" bottom="0.75" header="0.30" footer="0.30"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageMargins bottom="0.75" footer="0.30" header="0.30" left="0.70" right="0.70" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView zoomScale="399" workbookViewId="0">
+    <sheetView workbookViewId="0" zoomScale="399">
       <selection activeCell="C1" sqref="C1:D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.000000" customHeight="1"/>
+  <sheetFormatPr customHeight="1" defaultRowHeight="15.000000"/>
   <cols>
-    <col min="4" max="4" width="12.63000011" customWidth="1" outlineLevel="0"/>
+    <col min="4" max="4" customWidth="true" width="12.63000011" collapsed="true" outlineLevel="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16.500000">
+    <row ht="16.500000" r="1" spans="1:4">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
@@ -1540,7 +1590,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="16.500000">
+    <row ht="16.500000" r="2" spans="1:4">
       <c r="A2" s="0">
         <v>1</v>
       </c>
@@ -1554,7 +1604,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="16.500000">
+    <row ht="16.500000" r="3" spans="1:4">
       <c r="A3" s="0">
         <v>2</v>
       </c>
@@ -1570,58 +1620,58 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.70" right="0.70" top="0.75" bottom="0.75" header="0.30" footer="0.30"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageMargins bottom="0.75" footer="0.30" header="0.30" left="0.70" right="0.70" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView zoomScale="400" workbookViewId="0">
+    <sheetView workbookViewId="0" zoomScale="400">
       <selection activeCell="A4" sqref="A4:XFD5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.000000" customHeight="1"/>
+  <sheetFormatPr customHeight="1" defaultRowHeight="15.000000"/>
   <sheetData>
-    <row r="1" spans="1:1" ht="16.500000">
+    <row ht="16.500000" r="1" spans="1:1">
       <c r="A1" s="0" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="16.500000">
+    <row ht="16.500000" r="2" spans="1:1">
       <c r="A2" s="0" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="16.500000">
+    <row ht="16.500000" r="3" spans="1:1">
       <c r="A3" s="0" t="s">
         <v>23</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.70" right="0.70" top="0.75" bottom="0.75" header="0.30" footer="0.30"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageMargins bottom="0.75" footer="0.30" header="0.30" left="0.70" right="0.70" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView zoomScale="356" workbookViewId="0">
+    <sheetView workbookViewId="0" zoomScale="356">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.000000" customHeight="1"/>
+  <sheetFormatPr customHeight="1" defaultRowHeight="15.000000"/>
   <cols>
-    <col min="2" max="2" width="18.37999916" customWidth="1" outlineLevel="0"/>
-    <col min="4" max="4" width="33.88000107" customWidth="1" outlineLevel="0"/>
+    <col min="2" max="2" customWidth="true" width="18.37999916" collapsed="true" outlineLevel="0"/>
+    <col min="4" max="4" customWidth="true" width="33.88000107" collapsed="true" outlineLevel="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16.500000">
+    <row ht="16.500000" r="1" spans="1:4">
       <c r="A1" s="2" t="s">
         <v>67</v>
       </c>
@@ -1635,7 +1685,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="16.500000">
+    <row ht="16.500000" r="2" spans="1:4">
       <c r="A2" s="0">
         <v>0</v>
       </c>
@@ -1649,7 +1699,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="16.500000">
+    <row ht="16.500000" r="3" spans="1:4">
       <c r="A3" s="0">
         <v>1</v>
       </c>
@@ -1663,7 +1713,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="16.500000">
+    <row ht="16.500000" r="4" spans="1:4">
       <c r="A4" s="0">
         <v>2</v>
       </c>
@@ -1679,24 +1729,24 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.70" right="0.70" top="0.75" bottom="0.75" header="0.30" footer="0.30"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageMargins bottom="0.75" footer="0.30" header="0.30" left="0.70" right="0.70" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView zoomScale="385" workbookViewId="0">
+    <sheetView workbookViewId="0" zoomScale="385">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.500000" customHeight="1"/>
+  <sheetFormatPr customHeight="1" defaultRowHeight="16.500000"/>
   <cols>
-    <col min="2" max="2" width="14.25500011" customWidth="1" outlineLevel="0"/>
-    <col min="3" max="3" width="10.63000011" customWidth="1" outlineLevel="0"/>
-    <col min="5" max="5" width="31.25499916" customWidth="1" outlineLevel="0"/>
+    <col min="2" max="2" customWidth="true" width="14.25500011" collapsed="true" outlineLevel="0"/>
+    <col min="3" max="3" customWidth="true" width="10.63000011" collapsed="true" outlineLevel="0"/>
+    <col min="5" max="5" customWidth="true" width="31.25499916" collapsed="true" outlineLevel="0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1767,25 +1817,382 @@
         <v>31</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" t="s">
+        <v>98</v>
+      </c>
+      <c r="E5" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" t="s">
+        <v>115</v>
+      </c>
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" t="s">
+        <v>98</v>
+      </c>
+      <c r="E6" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" t="s">
+        <v>100</v>
+      </c>
+      <c r="E7" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" t="s">
+        <v>115</v>
+      </c>
+      <c r="C8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" t="s">
+        <v>98</v>
+      </c>
+      <c r="E8" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" t="s">
+        <v>115</v>
+      </c>
+      <c r="C9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" t="s">
+        <v>98</v>
+      </c>
+      <c r="E9" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" t="s">
+        <v>115</v>
+      </c>
+      <c r="C10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" t="s">
+        <v>98</v>
+      </c>
+      <c r="E10" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" t="s">
+        <v>115</v>
+      </c>
+      <c r="C11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" t="s">
+        <v>98</v>
+      </c>
+      <c r="E11" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" t="s">
+        <v>115</v>
+      </c>
+      <c r="C12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" t="s">
+        <v>98</v>
+      </c>
+      <c r="E12" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" t="s">
+        <v>115</v>
+      </c>
+      <c r="C13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" t="s">
+        <v>98</v>
+      </c>
+      <c r="E13" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" t="s">
+        <v>115</v>
+      </c>
+      <c r="C14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" t="s">
+        <v>100</v>
+      </c>
+      <c r="E14" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" t="s">
+        <v>115</v>
+      </c>
+      <c r="C15" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" t="s">
+        <v>98</v>
+      </c>
+      <c r="E15" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" t="s">
+        <v>115</v>
+      </c>
+      <c r="C16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" t="s">
+        <v>98</v>
+      </c>
+      <c r="E16" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" t="s">
+        <v>115</v>
+      </c>
+      <c r="C17" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" t="s">
+        <v>98</v>
+      </c>
+      <c r="E17" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" t="s">
+        <v>115</v>
+      </c>
+      <c r="C18" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" t="s">
+        <v>98</v>
+      </c>
+      <c r="E18" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" t="s">
+        <v>115</v>
+      </c>
+      <c r="C19" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" t="s">
+        <v>98</v>
+      </c>
+      <c r="E19" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" t="s">
+        <v>115</v>
+      </c>
+      <c r="C20" t="s">
+        <v>22</v>
+      </c>
+      <c r="D20" t="s">
+        <v>98</v>
+      </c>
+      <c r="E20" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" t="s">
+        <v>115</v>
+      </c>
+      <c r="C21" t="s">
+        <v>22</v>
+      </c>
+      <c r="D21" t="s">
+        <v>100</v>
+      </c>
+      <c r="E21" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" t="s">
+        <v>115</v>
+      </c>
+      <c r="C22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D22" t="s">
+        <v>98</v>
+      </c>
+      <c r="E22" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>33</v>
+      </c>
+      <c r="B23" t="s">
+        <v>115</v>
+      </c>
+      <c r="C23" t="s">
+        <v>22</v>
+      </c>
+      <c r="D23" t="s">
+        <v>98</v>
+      </c>
+      <c r="E23" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>33</v>
+      </c>
+      <c r="B24" t="s">
+        <v>115</v>
+      </c>
+      <c r="C24" t="s">
+        <v>22</v>
+      </c>
+      <c r="D24" t="s">
+        <v>98</v>
+      </c>
+      <c r="E24" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>33</v>
+      </c>
+      <c r="B25" t="s">
+        <v>115</v>
+      </c>
+      <c r="C25" t="s">
+        <v>22</v>
+      </c>
+      <c r="D25" t="s">
+        <v>98</v>
+      </c>
+      <c r="E25" t="s">
+        <v>203</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.70" right="0.70" top="0.75" bottom="0.75" header="0.30" footer="0.30"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageMargins bottom="0.75" footer="0.30" header="0.30" left="0.70" right="0.70" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="400" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0" zoomScale="400">
       <selection activeCell="B6" sqref="B6:D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.500000" customHeight="1"/>
+  <sheetFormatPr customHeight="1" defaultRowHeight="16.500000"/>
   <cols>
-    <col min="1" max="1" width="8.00500011" customWidth="1" outlineLevel="0"/>
-    <col min="4" max="4" width="31.25499916" customWidth="1" outlineLevel="0"/>
+    <col min="1" max="1" customWidth="true" width="8.00500011" collapsed="true" outlineLevel="0"/>
+    <col min="4" max="4" customWidth="true" width="31.25499916" collapsed="true" outlineLevel="0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1858,27 +2265,153 @@
         <v>180</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
+        <v>181</v>
+      </c>
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" t="s">
+        <v>181</v>
+      </c>
+      <c r="C9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" t="s">
+        <v>57</v>
+      </c>
+      <c r="C11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" t="s">
+        <v>181</v>
+      </c>
+      <c r="C12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" t="s">
+        <v>57</v>
+      </c>
+      <c r="C13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" t="s">
+        <v>57</v>
+      </c>
+      <c r="C14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" t="s">
+        <v>202</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.70" right="0.70" top="0.75" bottom="0.75" header="0.30" footer="0.30"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageMargins bottom="0.75" footer="0.30" header="0.30" left="0.70" right="0.70" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView zoomScale="400" workbookViewId="0">
+    <sheetView workbookViewId="0" zoomScale="400">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.000000" customHeight="1"/>
+  <sheetFormatPr customHeight="1" defaultRowHeight="15.000000"/>
   <cols>
-    <col min="2" max="2" width="16.13000011" customWidth="1" outlineLevel="0"/>
+    <col min="2" max="2" customWidth="true" width="16.13000011" collapsed="true" outlineLevel="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.500000">
+    <row ht="16.500000" r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1886,7 +2419,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="16.500000">
+    <row ht="16.500000" r="2" spans="1:2">
       <c r="A2" s="0">
         <v>1</v>
       </c>
@@ -1894,7 +2427,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="16.500000">
+    <row ht="16.500000" r="3" spans="1:2">
       <c r="A3" s="0">
         <v>2</v>
       </c>
@@ -1902,7 +2435,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="16.500000">
+    <row ht="16.500000" r="4" spans="1:2">
       <c r="A4" s="0">
         <v>3</v>
       </c>
@@ -1912,7 +2445,7 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.70" right="0.70" top="0.75" bottom="0.75" header="0.30" footer="0.30"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageMargins bottom="0.75" footer="0.30" header="0.30" left="0.70" right="0.70" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>
 </file>
</xml_diff>